<commit_message>
thesis - 5. all diagrams added
</commit_message>
<xml_diff>
--- a/hu.bme.mit.vmdistribution.app/doc/perf_anal/result.xlsx
+++ b/hu.bme.mit.vmdistribution.app/doc/perf_anal/result.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="63">
   <si>
     <t>distribution to all fast machines</t>
   </si>
@@ -135,33 +135,6 @@
     <t>leggyorsabb</t>
   </si>
   <si>
-    <t>pc39</t>
-  </si>
-  <si>
-    <t>pc05</t>
-  </si>
-  <si>
-    <t>pc07</t>
-  </si>
-  <si>
-    <t>pc11</t>
-  </si>
-  <si>
-    <t>pc19</t>
-  </si>
-  <si>
-    <t>pc20</t>
-  </si>
-  <si>
-    <t>pc21</t>
-  </si>
-  <si>
-    <t>pc27</t>
-  </si>
-  <si>
-    <t>pc38</t>
-  </si>
-  <si>
     <t>diff</t>
   </si>
   <si>
@@ -202,6 +175,36 @@
   </si>
   <si>
     <t>Átlag</t>
+  </si>
+  <si>
+    <t>10 gép</t>
+  </si>
+  <si>
+    <t>25 gép</t>
+  </si>
+  <si>
+    <t>PC05</t>
+  </si>
+  <si>
+    <t>PC07</t>
+  </si>
+  <si>
+    <t>PC11</t>
+  </si>
+  <si>
+    <t>PC19</t>
+  </si>
+  <si>
+    <t>PC20</t>
+  </si>
+  <si>
+    <t>PC21</t>
+  </si>
+  <si>
+    <t>PC27</t>
+  </si>
+  <si>
+    <t>PC38</t>
   </si>
 </sst>
 </file>
@@ -210,7 +213,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0;\ \a\s\d"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -248,13 +251,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -461,11 +470,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="101340288"/>
-        <c:axId val="101342208"/>
+        <c:axId val="98329728"/>
+        <c:axId val="98331648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="101340288"/>
+        <c:axId val="98329728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -501,7 +510,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="101342208"/>
+        <c:crossAx val="98331648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -509,7 +518,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101342208"/>
+        <c:axId val="98331648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="500"/>
@@ -547,7 +556,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101340288"/>
+        <c:crossAx val="98329728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -584,6 +593,21 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="hu-HU"/>
+              <a:t>Legkésőbb végző gépek</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
@@ -594,10 +618,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.32985214348206476"/>
-          <c:y val="0.24323636628754738"/>
-          <c:w val="0.38860258092738409"/>
-          <c:h val="0.64767096821230674"/>
+          <c:x val="0.27224753587134737"/>
+          <c:y val="0.2397561294054224"/>
+          <c:w val="0.51884180768306498"/>
+          <c:h val="0.65850711213189861"/>
         </c:manualLayout>
       </c:layout>
       <c:pieChart>
@@ -683,6 +707,13 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:solidFill>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:solidFill>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -706,12 +737,37 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="hu-HU"/>
+              <a:t>Leghamarabb végző gépek</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.26561752250708259"/>
+          <c:y val="0.24096865910880078"/>
+          <c:w val="0.51181122194759499"/>
+          <c:h val="0.65612973669608177"/>
+        </c:manualLayout>
+      </c:layout>
       <c:pieChart>
         <c:varyColors val="1"/>
         <c:ser>
@@ -732,31 +788,31 @@
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>pc05</c:v>
+                  <c:v>PC05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>pc07</c:v>
+                  <c:v>PC07</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>pc11</c:v>
+                  <c:v>PC11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>pc19</c:v>
+                  <c:v>PC19</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>pc20</c:v>
+                  <c:v>PC20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>pc21</c:v>
+                  <c:v>PC21</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>pc27</c:v>
+                  <c:v>PC27</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>pc38</c:v>
+                  <c:v>PC38</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>pc39</c:v>
+                  <c:v>PC39</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -819,6 +875,13 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:solidFill>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:solidFill>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -964,11 +1027,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="45855104"/>
-        <c:axId val="45856640"/>
+        <c:axId val="103946112"/>
+        <c:axId val="103952384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="45855104"/>
+        <c:axId val="103946112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -996,7 +1059,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45856640"/>
+        <c:crossAx val="103952384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1004,7 +1067,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45856640"/>
+        <c:axId val="103952384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="700"/>
@@ -1050,7 +1113,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45855104"/>
+        <c:crossAx val="103946112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1106,16 +1169,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>16774</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>9548</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>41414</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>182218</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>319275</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>85748</xdr:rowOff>
+      <xdr:rowOff>173934</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1136,16 +1199,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>316531</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>9102</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>8284</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>182217</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>10417</xdr:colOff>
+      <xdr:colOff>3312</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>85302</xdr:rowOff>
+      <xdr:rowOff>173934</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1166,16 +1229,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>249620</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>155685</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>191642</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>97708</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>367861</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>41385</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>273326</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>24848</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1484,10 +1547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U68"/>
+  <dimension ref="A1:U93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="M39" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="T57" sqref="T57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1677,7 +1740,7 @@
         <v>19</v>
       </c>
       <c r="G11" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="H11">
         <v>359</v>
@@ -1772,15 +1835,15 @@
         <v>22</v>
       </c>
       <c r="E23" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="F23" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B24">
         <v>310</v>
@@ -1799,7 +1862,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B25">
         <v>289</v>
@@ -1818,7 +1881,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B26">
         <v>315</v>
@@ -1837,7 +1900,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B27" s="4">
         <f>AVERAGE(B24:B26)</f>
@@ -1850,7 +1913,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B28" t="str">
         <f>A28</f>
@@ -1861,7 +1924,7 @@
         <v>5.4794520547945202E-2</v>
       </c>
       <c r="F28" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1995,7 +2058,7 @@
         <v>36.18</v>
       </c>
       <c r="G39" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="H39">
         <v>1</v>
@@ -2009,7 +2072,7 @@
         <v>19.09</v>
       </c>
       <c r="G40" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="H40">
         <v>4</v>
@@ -2023,7 +2086,7 @@
         <v>36.85</v>
       </c>
       <c r="G41" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="H41">
         <v>1</v>
@@ -2037,7 +2100,7 @@
         <v>38.29</v>
       </c>
       <c r="G42" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H42">
         <v>4</v>
@@ -2051,7 +2114,7 @@
         <v>29.74</v>
       </c>
       <c r="G43" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H43">
         <v>1</v>
@@ -2226,7 +2289,7 @@
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="G60" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="H60">
         <v>2</v>
@@ -2238,11 +2301,11 @@
         <v>38.592499999999994</v>
       </c>
       <c r="C61">
-        <f t="shared" ref="B61:C61" si="2">AVERAGE(C36:C59)</f>
+        <f t="shared" ref="C61" si="2">AVERAGE(C36:C59)</f>
         <v>27.562083333333334</v>
       </c>
       <c r="G61" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="H61">
         <v>1</v>
@@ -2250,7 +2313,7 @@
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="G62" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="H62">
         <v>1</v>
@@ -2258,7 +2321,7 @@
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="G63" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="H63">
         <v>1</v>
@@ -2266,45 +2329,271 @@
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="G64" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="H64">
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G65" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="H65">
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G66" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="H66">
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G67" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="H67">
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G68" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="H68">
         <v>1</v>
       </c>
     </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H78" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I78" s="6"/>
+      <c r="J78" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K78" s="6"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H79" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I79" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J79" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K79" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>1</v>
+      </c>
+      <c r="B80" t="s">
+        <v>8</v>
+      </c>
+      <c r="C80" t="s">
+        <v>9</v>
+      </c>
+      <c r="D80" t="s">
+        <v>5</v>
+      </c>
+      <c r="G80" t="s">
+        <v>2</v>
+      </c>
+      <c r="H80">
+        <v>85</v>
+      </c>
+      <c r="I80">
+        <v>86</v>
+      </c>
+      <c r="J80">
+        <v>80</v>
+      </c>
+      <c r="K80">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>86</v>
+      </c>
+      <c r="C81">
+        <v>81</v>
+      </c>
+      <c r="D81" t="s">
+        <v>14</v>
+      </c>
+      <c r="G81" t="s">
+        <v>3</v>
+      </c>
+      <c r="H81">
+        <v>178</v>
+      </c>
+      <c r="I81">
+        <v>340</v>
+      </c>
+      <c r="J81">
+        <v>167</v>
+      </c>
+      <c r="K81">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <v>340</v>
+      </c>
+      <c r="C82">
+        <v>333</v>
+      </c>
+      <c r="D82" t="s">
+        <v>14</v>
+      </c>
+      <c r="G82" t="s">
+        <v>4</v>
+      </c>
+      <c r="H82">
+        <v>293</v>
+      </c>
+      <c r="I82">
+        <v>310</v>
+      </c>
+      <c r="J82">
+        <v>270</v>
+      </c>
+      <c r="K82">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B83">
+        <v>310</v>
+      </c>
+      <c r="C83">
+        <v>297</v>
+      </c>
+      <c r="D83" t="s">
+        <v>14</v>
+      </c>
+      <c r="G83" t="s">
+        <v>6</v>
+      </c>
+      <c r="H83">
+        <v>563</v>
+      </c>
+      <c r="I83">
+        <v>442</v>
+      </c>
+      <c r="J83">
+        <v>516</v>
+      </c>
+      <c r="K83">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B84">
+        <v>442</v>
+      </c>
+      <c r="C84">
+        <v>361</v>
+      </c>
+      <c r="D84" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>1</v>
+      </c>
+      <c r="B89" t="s">
+        <v>8</v>
+      </c>
+      <c r="C89" t="s">
+        <v>20</v>
+      </c>
+      <c r="D89" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>2</v>
+      </c>
+      <c r="B90">
+        <v>85</v>
+      </c>
+      <c r="C90">
+        <v>80</v>
+      </c>
+      <c r="D90" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>3</v>
+      </c>
+      <c r="B91">
+        <v>178</v>
+      </c>
+      <c r="C91">
+        <v>167</v>
+      </c>
+      <c r="D91" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>4</v>
+      </c>
+      <c r="B92">
+        <v>293</v>
+      </c>
+      <c r="C92">
+        <v>270</v>
+      </c>
+      <c r="D92" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>6</v>
+      </c>
+      <c r="B93">
+        <v>563</v>
+      </c>
+      <c r="C93">
+        <v>516</v>
+      </c>
+      <c r="D93" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="H78:I78"/>
+    <mergeCell ref="J78:K78"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>